<commit_message>
Received orders from mouser and digikey
</commit_message>
<xml_diff>
--- a/orders/order-tracking.xlsx
+++ b/orders/order-tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-hardware/orders/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cam/flora-GIT/flora-hardware/orders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_F25DC773A252ABDACC10489A291A57685BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D50AD24-3A5E-43B1-8D2C-BBFED1356C25}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A0D306-4CD3-6343-9812-E933509873A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30315" yWindow="1515" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Order #</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>JLC was unsure about the footprints for J8 and J7 because of the large solder mask opening. Told them to continue per the gerber -AH</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Friday,Octoder 18, 2024</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
@@ -183,16 +192,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F239E3FA-E447-4B99-A348-1DC7CF1A0F20}" name="Table1" displayName="Table1" ref="B3:H11" totalsRowShown="0">
-  <autoFilter ref="B3:H11" xr:uid="{F239E3FA-E447-4B99-A348-1DC7CF1A0F20}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F239E3FA-E447-4B99-A348-1DC7CF1A0F20}" name="Table1" displayName="Table1" ref="B3:I11" totalsRowShown="0">
+  <autoFilter ref="B3:I11" xr:uid="{F239E3FA-E447-4B99-A348-1DC7CF1A0F20}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6AAD179A-0F64-4A68-A6DE-B5FC327D7F8D}" name="Order #"/>
-    <tableColumn id="2" xr3:uid="{3541061D-16F5-4BCE-9ABF-7488DAAB4A49}" name="Cost" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3541061D-16F5-4BCE-9ABF-7488DAAB4A49}" name="Cost" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{2927EC20-DA80-4FFE-8E26-F88581B56D2A}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{BA13A7D8-4DCF-4CBA-B541-CFA1DA51DFC5}" name="Date Submitted" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{E6D40592-E467-4561-9221-00BE163E209D}" name="Revision Date (?)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{512FF338-EE33-45EF-9E5B-97CCB36C4767}" name="Date Approved" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{2960DCF8-EA79-4F66-88E1-B8FFAD15EE77}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BA13A7D8-4DCF-4CBA-B541-CFA1DA51DFC5}" name="Date Submitted" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{E6D40592-E467-4561-9221-00BE163E209D}" name="Revision Date (?)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{512FF338-EE33-45EF-9E5B-97CCB36C4767}" name="Date Approved" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{6E0B6201-379C-F44C-BB9A-A0BE28DEDA01}" name="Received" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{2960DCF8-EA79-4F66-88E1-B8FFAD15EE77}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -203,12 +213,12 @@
   <autoFilter ref="B15:H23" xr:uid="{734F5A1B-1E7E-42A4-B30D-3818CF329E28}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0AB9CF5F-18A0-43AC-BB6F-25ADB58C0075}" name="Order #"/>
-    <tableColumn id="2" xr3:uid="{C08CE223-DD40-4E46-A893-662F4B0D40D6}" name="Estimated Cost" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C08CE223-DD40-4E46-A893-662F4B0D40D6}" name="Estimated Cost" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{5155CF55-244E-439C-BFD1-FC651D2A3336}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{B0C24102-4CCF-47B2-8A75-57547BDFA69F}" name="Date Submitted" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F7C0AD5A-1A01-4E92-8EE1-367603B75601}" name="Revision Date (?)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{35677311-7B5E-4D65-8A54-5F27C4844BD6}" name="Date Approved" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{6D74F58A-2DD8-43A0-BB6F-DACAFB8AB005}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B0C24102-4CCF-47B2-8A75-57547BDFA69F}" name="Date Submitted" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F7C0AD5A-1A01-4E92-8EE1-367603B75601}" name="Revision Date (?)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{35677311-7B5E-4D65-8A54-5F27C4844BD6}" name="Date Approved" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{6D74F58A-2DD8-43A0-BB6F-DACAFB8AB005}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -477,29 +487,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="63.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -519,10 +530,13 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -543,8 +557,9 @@
         <v>45552</v>
       </c>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -564,9 +579,10 @@
       <c r="G5" s="3">
         <v>45558</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:9" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -586,11 +602,14 @@
       <c r="G6" s="1">
         <v>45580</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
@@ -598,8 +617,9 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
@@ -607,8 +627,9 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
@@ -616,8 +637,9 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
@@ -625,8 +647,9 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
@@ -634,13 +657,14 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -663,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>1</v>
       </c>
@@ -686,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1" t="s">
@@ -695,7 +719,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C18" s="2"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
@@ -704,7 +728,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
@@ -713,7 +737,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C20" s="2"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
@@ -722,7 +746,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
@@ -731,7 +755,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C22" s="2"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
@@ -740,7 +764,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">

</xml_diff>